<commit_message>
Ajuste de motores en escaleta MA_11_04_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion04/Escaleta_MA_11_04_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion04/Escaleta_MA_11_04_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\Matematicas\fuentes\contenidos\grado11\guion04\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado11\guion04\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$32</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -845,13 +845,13 @@
     <t>Recurso M5A-04</t>
   </si>
   <si>
-    <t>Recurso M4A-01</t>
-  </si>
-  <si>
-    <t>Recurso M4A-02</t>
-  </si>
-  <si>
-    <t>Recurso M4A-03</t>
+    <t>Recurso M102AB-02</t>
+  </si>
+  <si>
+    <t>Recurso M102AB-03</t>
+  </si>
+  <si>
+    <t>Recurso M102AB-04</t>
   </si>
 </sst>
 </file>
@@ -1161,34 +1161,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1228,6 +1210,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1537,127 +1537,127 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T27" sqref="T27"/>
+      <selection pane="bottomLeft" activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.4" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.4" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.86328125" customWidth="1"/>
-    <col min="2" max="2" width="16.86328125" customWidth="1"/>
-    <col min="3" max="3" width="26.73046875" customWidth="1"/>
-    <col min="4" max="4" width="26.1328125" customWidth="1"/>
-    <col min="5" max="5" width="42.59765625" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="42.5703125" customWidth="1"/>
     <col min="6" max="6" width="8" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.265625" customWidth="1"/>
-    <col min="8" max="8" width="8.3984375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.73046875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.28515625" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="49" customWidth="1"/>
-    <col min="11" max="11" width="13.265625" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" customWidth="1"/>
     <col min="12" max="12" width="11" customWidth="1"/>
-    <col min="13" max="13" width="6.73046875" customWidth="1"/>
-    <col min="14" max="14" width="7.73046875" customWidth="1"/>
-    <col min="15" max="15" width="54.1328125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="11.3984375" style="6" customWidth="1"/>
-    <col min="17" max="17" width="7.73046875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="7.86328125" customWidth="1"/>
-    <col min="19" max="19" width="10.3984375" customWidth="1"/>
-    <col min="20" max="20" width="17.1328125" customWidth="1"/>
-    <col min="21" max="21" width="13.59765625" customWidth="1"/>
+    <col min="13" max="13" width="6.7109375" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" customWidth="1"/>
+    <col min="15" max="15" width="54.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" style="6" customWidth="1"/>
+    <col min="17" max="17" width="7.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="7.85546875" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" customWidth="1"/>
+    <col min="20" max="20" width="17.140625" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="55" t="s">
+      <c r="G1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="I1" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="59" t="s">
+      <c r="J1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="57" t="s">
+      <c r="K1" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="55" t="s">
+      <c r="L1" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="61" t="s">
+      <c r="M1" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="61"/>
-      <c r="O1" s="41" t="s">
+      <c r="N1" s="55"/>
+      <c r="O1" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="41" t="s">
+      <c r="P1" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="43" t="s">
+      <c r="Q1" s="58" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="47" t="s">
+      <c r="R1" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="43" t="s">
+      <c r="S1" s="58" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="45" t="s">
+      <c r="T1" s="60" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="43" t="s">
+      <c r="U1" s="58" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="54"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="56"/>
+    <row r="2" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="48"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="50"/>
       <c r="M2" s="5" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="42"/>
-      <c r="P2" s="42"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="48"/>
-      <c r="S2" s="44"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="44"/>
-    </row>
-    <row r="3" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="63"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="61"/>
+      <c r="U2" s="59"/>
+    </row>
+    <row r="3" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>15</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
@@ -1777,7 +1777,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>15</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="7" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
@@ -1936,7 +1936,7 @@
       </c>
       <c r="M7" s="27"/>
       <c r="N7" s="27" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="O7" s="23" t="s">
         <v>239</v>
@@ -1954,7 +1954,7 @@
         <v>158</v>
       </c>
       <c r="T7" s="21" t="s">
-        <v>273</v>
+        <v>217</v>
       </c>
       <c r="U7" s="19" t="s">
         <v>159</v>
@@ -1963,7 +1963,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>15</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="9" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="10" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>15</v>
       </c>
@@ -2146,7 +2146,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>15</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="12" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>15</v>
       </c>
@@ -2244,7 +2244,7 @@
       </c>
       <c r="M12" s="27"/>
       <c r="N12" s="27" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="O12" s="23" t="s">
         <v>242</v>
@@ -2262,7 +2262,7 @@
         <v>158</v>
       </c>
       <c r="T12" s="21" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="U12" s="19" t="s">
         <v>159</v>
@@ -2271,7 +2271,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="13" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>15</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="14" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>15</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="15" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>15</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="16" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:22" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>15</v>
       </c>
@@ -2491,7 +2491,7 @@
       </c>
       <c r="M16" s="27"/>
       <c r="N16" s="27" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="O16" s="23" t="s">
         <v>251</v>
@@ -2509,7 +2509,7 @@
         <v>158</v>
       </c>
       <c r="T16" s="21" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="U16" s="19" t="s">
         <v>159</v>
@@ -2518,7 +2518,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="17" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="18" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>15</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="19" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>15</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="20" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>15</v>
       </c>
@@ -2762,7 +2762,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="21" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>15</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="22" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>15</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="23" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>15</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="24" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>15</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="25" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>15</v>
       </c>
@@ -3067,7 +3067,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="26" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>15</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="27" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>15</v>
       </c>
@@ -3189,7 +3189,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="28" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>15</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="29" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>15</v>
       </c>
@@ -3305,13 +3305,13 @@
         <v>158</v>
       </c>
       <c r="T29" s="21" t="s">
-        <v>217</v>
+        <v>275</v>
       </c>
       <c r="U29" s="19" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="30" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="37" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="37" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>15</v>
       </c>
@@ -13759,7 +13759,7 @@
       <c r="XFB30" s="38"/>
       <c r="XFD30" s="40"/>
     </row>
-    <row r="31" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>15</v>
       </c>
@@ -13820,7 +13820,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="32" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:2048 2054:3072 3074:4094 4100:6140 6146:10239 10241:11263 11265:13312 13318:14336 14338:15358 15364:16384" s="4" customFormat="1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>15</v>
       </c>
@@ -13881,187 +13881,187 @@
         <v>159</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:1" ht="12.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>115</v>
       </c>
@@ -14071,6 +14071,12 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -14085,12 +14091,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="V7" r:id="rId1"/>
@@ -14101,7 +14101,7 @@
   <pageSetup orientation="portrait" r:id="rId4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$E$14:$E$48</xm:f>
@@ -14146,27 +14146,27 @@
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.86328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.86328125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="34" style="2" customWidth="1"/>
-    <col min="5" max="5" width="34.86328125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.59765625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" style="2" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.86328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.73046875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="15.59765625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" style="2" customWidth="1"/>
     <col min="12" max="12" width="17" style="2" customWidth="1"/>
-    <col min="13" max="13" width="11.3984375" style="2"/>
-    <col min="14" max="14" width="24.265625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="69.86328125" style="2" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.3984375" style="2"/>
+    <col min="13" max="13" width="11.42578125" style="2"/>
+    <col min="14" max="14" width="24.28515625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="69.85546875" style="2" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -14183,7 +14183,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -14207,7 +14207,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -14226,7 +14226,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -14245,7 +14245,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
@@ -14261,7 +14261,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
@@ -14278,7 +14278,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
@@ -14295,7 +14295,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -14310,7 +14310,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -14325,7 +14325,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -14340,7 +14340,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -14355,7 +14355,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -14370,7 +14370,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -14385,7 +14385,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -14400,7 +14400,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -14415,7 +14415,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -14430,7 +14430,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="2" t="s">
@@ -14444,7 +14444,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="2" t="s">
@@ -14458,7 +14458,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="2" t="s">
@@ -14472,7 +14472,7 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="2" t="s">
@@ -14486,7 +14486,7 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -14501,7 +14501,7 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -14516,7 +14516,7 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -14531,7 +14531,7 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -14546,7 +14546,7 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -14561,7 +14561,7 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -14576,7 +14576,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -14591,7 +14591,7 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -14606,7 +14606,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -14621,7 +14621,7 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
     </row>
-    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -14636,7 +14636,7 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -14651,7 +14651,7 @@
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
     </row>
-    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -14666,7 +14666,7 @@
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -14681,7 +14681,7 @@
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -14696,7 +14696,7 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -14711,7 +14711,7 @@
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -14726,7 +14726,7 @@
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -14741,7 +14741,7 @@
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -14756,7 +14756,7 @@
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
     </row>
-    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -14771,7 +14771,7 @@
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -14786,7 +14786,7 @@
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
     </row>
-    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -14801,7 +14801,7 @@
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -14816,7 +14816,7 @@
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -14831,7 +14831,7 @@
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -14846,7 +14846,7 @@
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -14861,7 +14861,7 @@
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -14876,7 +14876,7 @@
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -14891,7 +14891,7 @@
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
     </row>
-    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
@@ -14906,7 +14906,7 @@
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -14918,7 +14918,7 @@
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
@@ -14930,7 +14930,7 @@
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
     </row>
-    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -14943,7 +14943,7 @@
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
     </row>
-    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
@@ -14956,7 +14956,7 @@
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -14969,7 +14969,7 @@
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
     </row>
-    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -14982,7 +14982,7 @@
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
     </row>
-    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
@@ -14995,7 +14995,7 @@
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
     </row>
-    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
@@ -15008,7 +15008,7 @@
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
     </row>
-    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
@@ -15021,7 +15021,7 @@
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
     </row>
-    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -15034,7 +15034,7 @@
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
     </row>
-    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
@@ -15047,7 +15047,7 @@
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
     </row>
-    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
@@ -15060,7 +15060,7 @@
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
     </row>
-    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -15073,7 +15073,7 @@
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
     </row>
-    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
@@ -15086,7 +15086,7 @@
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
     </row>
-    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
@@ -15099,7 +15099,7 @@
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
     </row>
-    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
@@ -15112,7 +15112,7 @@
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
     </row>
-    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
@@ -15125,7 +15125,7 @@
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
     </row>
-    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
@@ -15138,7 +15138,7 @@
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
@@ -15151,7 +15151,7 @@
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
     </row>
-    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
@@ -15164,7 +15164,7 @@
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
@@ -15177,7 +15177,7 @@
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
     </row>
-    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
@@ -15190,7 +15190,7 @@
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
     </row>
-    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -15204,7 +15204,7 @@
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -15218,7 +15218,7 @@
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -15232,7 +15232,7 @@
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -15246,7 +15246,7 @@
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
     </row>
-    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -15260,7 +15260,7 @@
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -15274,7 +15274,7 @@
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
     </row>
-    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -15288,7 +15288,7 @@
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
     </row>
-    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -15302,7 +15302,7 @@
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
     </row>
-    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -15316,7 +15316,7 @@
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
     </row>
-    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -15330,7 +15330,7 @@
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
     </row>
-    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -15344,7 +15344,7 @@
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
     </row>
-    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -15358,7 +15358,7 @@
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
     </row>
-    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -15372,7 +15372,7 @@
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
     </row>
-    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -15386,7 +15386,7 @@
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
     </row>
-    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
@@ -15400,7 +15400,7 @@
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
     </row>
-    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -15414,7 +15414,7 @@
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
     </row>
-    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -15428,7 +15428,7 @@
       <c r="K87" s="3"/>
       <c r="L87" s="3"/>
     </row>
-    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -15442,7 +15442,7 @@
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
     </row>
-    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -15456,7 +15456,7 @@
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
     </row>
-    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -15470,7 +15470,7 @@
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
     </row>
-    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
@@ -15484,7 +15484,7 @@
       <c r="K91" s="3"/>
       <c r="L91" s="3"/>
     </row>
-    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -15498,7 +15498,7 @@
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
     </row>
-    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -15512,7 +15512,7 @@
       <c r="K93" s="3"/>
       <c r="L93" s="3"/>
     </row>
-    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -15526,7 +15526,7 @@
       <c r="K94" s="3"/>
       <c r="L94" s="3"/>
     </row>
-    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
@@ -15540,7 +15540,7 @@
       <c r="K95" s="3"/>
       <c r="L95" s="3"/>
     </row>
-    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
@@ -15554,7 +15554,7 @@
       <c r="K96" s="3"/>
       <c r="L96" s="3"/>
     </row>
-    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
@@ -15568,7 +15568,7 @@
       <c r="K97" s="3"/>
       <c r="L97" s="3"/>
     </row>
-    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
@@ -15582,7 +15582,7 @@
       <c r="K98" s="3"/>
       <c r="L98" s="3"/>
     </row>
-    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
@@ -15596,7 +15596,7 @@
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
     </row>
-    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -15610,7 +15610,7 @@
       <c r="K100" s="3"/>
       <c r="L100" s="3"/>
     </row>
-    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -15624,7 +15624,7 @@
       <c r="K101" s="3"/>
       <c r="L101" s="3"/>
     </row>
-    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
@@ -15638,7 +15638,7 @@
       <c r="K102" s="3"/>
       <c r="L102" s="3"/>
     </row>
-    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -15652,7 +15652,7 @@
       <c r="K103" s="3"/>
       <c r="L103" s="3"/>
     </row>
-    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
@@ -15666,7 +15666,7 @@
       <c r="K104" s="3"/>
       <c r="L104" s="3"/>
     </row>
-    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
@@ -15680,7 +15680,7 @@
       <c r="K105" s="3"/>
       <c r="L105" s="3"/>
     </row>
-    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -15694,7 +15694,7 @@
       <c r="K106" s="3"/>
       <c r="L106" s="3"/>
     </row>
-    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -15708,7 +15708,7 @@
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
     </row>
-    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="3"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
@@ -15722,7 +15722,7 @@
       <c r="K108" s="3"/>
       <c r="L108" s="3"/>
     </row>
-    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="3"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
@@ -15736,7 +15736,7 @@
       <c r="K109" s="3"/>
       <c r="L109" s="3"/>
     </row>
-    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -15750,7 +15750,7 @@
       <c r="K110" s="3"/>
       <c r="L110" s="3"/>
     </row>
-    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
@@ -15764,7 +15764,7 @@
       <c r="K111" s="3"/>
       <c r="L111" s="3"/>
     </row>
-    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="3"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
@@ -15778,7 +15778,7 @@
       <c r="K112" s="3"/>
       <c r="L112" s="3"/>
     </row>
-    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -15792,7 +15792,7 @@
       <c r="K113" s="3"/>
       <c r="L113" s="3"/>
     </row>
-    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="3"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -15806,7 +15806,7 @@
       <c r="K114" s="3"/>
       <c r="L114" s="3"/>
     </row>
-    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="3"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
@@ -15820,7 +15820,7 @@
       <c r="K115" s="3"/>
       <c r="L115" s="3"/>
     </row>
-    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="3"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
@@ -15834,7 +15834,7 @@
       <c r="K116" s="3"/>
       <c r="L116" s="3"/>
     </row>
-    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="3"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
@@ -15848,7 +15848,7 @@
       <c r="K117" s="3"/>
       <c r="L117" s="3"/>
     </row>
-    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="3"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
@@ -15862,7 +15862,7 @@
       <c r="K118" s="3"/>
       <c r="L118" s="3"/>
     </row>
-    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="3"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
@@ -15876,7 +15876,7 @@
       <c r="K119" s="3"/>
       <c r="L119" s="3"/>
     </row>
-    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
@@ -15890,7 +15890,7 @@
       <c r="K120" s="3"/>
       <c r="L120" s="3"/>
     </row>
-    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="3"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
@@ -15904,7 +15904,7 @@
       <c r="K121" s="3"/>
       <c r="L121" s="3"/>
     </row>
-    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="3"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
@@ -15918,7 +15918,7 @@
       <c r="K122" s="3"/>
       <c r="L122" s="3"/>
     </row>
-    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
@@ -15932,7 +15932,7 @@
       <c r="K123" s="3"/>
       <c r="L123" s="3"/>
     </row>
-    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="3"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
@@ -15946,7 +15946,7 @@
       <c r="K124" s="3"/>
       <c r="L124" s="3"/>
     </row>
-    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="3"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
@@ -15960,7 +15960,7 @@
       <c r="K125" s="3"/>
       <c r="L125" s="3"/>
     </row>
-    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="3"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
@@ -15974,7 +15974,7 @@
       <c r="K126" s="3"/>
       <c r="L126" s="3"/>
     </row>
-    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="3"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -15988,7 +15988,7 @@
       <c r="K127" s="3"/>
       <c r="L127" s="3"/>
     </row>
-    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="3"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
@@ -16002,7 +16002,7 @@
       <c r="K128" s="3"/>
       <c r="L128" s="3"/>
     </row>
-    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="3"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
@@ -16016,7 +16016,7 @@
       <c r="K129" s="3"/>
       <c r="L129" s="3"/>
     </row>
-    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="3"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
@@ -16030,7 +16030,7 @@
       <c r="K130" s="3"/>
       <c r="L130" s="3"/>
     </row>
-    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="3"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
@@ -16044,7 +16044,7 @@
       <c r="K131" s="3"/>
       <c r="L131" s="3"/>
     </row>
-    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="3"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
@@ -16058,7 +16058,7 @@
       <c r="K132" s="3"/>
       <c r="L132" s="3"/>
     </row>
-    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="3"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>

</xml_diff>